<commit_message>
move save_nwaykshot func, complete step05
</commit_message>
<xml_diff>
--- a/metaX 예시코드 사용자 입력 정의.xlsx
+++ b/metaX 예시코드 사용자 입력 정의.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
   <si>
     <t>Predict</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -175,10 +175,6 @@
   </si>
   <si>
     <t xml:space="preserve">몇 번 학습한 모델을 불러올 것인지 입력, None이면 최종 학습한 모델 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>epochs_to_load_from</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -391,23 +387,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -692,7 +688,7 @@
   <dimension ref="B1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -705,13 +701,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -735,7 +731,7 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -747,15 +743,15 @@
         <v>19</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="7" t="s">
-        <v>60</v>
+      <c r="B5" s="12" t="s">
+        <v>59</v>
       </c>
       <c r="C5" s="3">
         <v>2</v>
@@ -774,7 +770,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="7"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="3">
         <v>3</v>
       </c>
@@ -792,17 +788,17 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="7"/>
-      <c r="C7" s="10">
+      <c r="B7" s="12"/>
+      <c r="C7" s="8">
         <v>4</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="10">
         <v>7</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="10" t="s">
         <v>24</v>
       </c>
       <c r="G7" s="5" t="s">
@@ -810,8 +806,8 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="7" t="s">
-        <v>61</v>
+      <c r="B8" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
@@ -823,14 +819,14 @@
         <v>5</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="7"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="3">
         <v>2</v>
       </c>
@@ -848,7 +844,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="7"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="3">
         <v>3</v>
       </c>
@@ -859,14 +855,14 @@
         <v>1E-3</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="7"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="3">
         <v>4</v>
       </c>
@@ -884,7 +880,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="7"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="3">
         <v>5</v>
       </c>
@@ -895,14 +891,14 @@
         <v>10</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="7"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="3">
         <v>6</v>
       </c>
@@ -920,25 +916,25 @@
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="7"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="3">
         <v>7</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="5">
         <v>10</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="7"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="3">
         <v>8</v>
       </c>
@@ -949,14 +945,14 @@
         <v>1</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="7"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="3">
         <v>9</v>
       </c>
@@ -967,89 +963,89 @@
         <v>50</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="7"/>
-      <c r="C17" s="9">
+      <c r="B17" s="12"/>
+      <c r="C17" s="7">
         <v>10</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E17" s="5">
         <v>1</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="7" t="s">
-        <v>62</v>
+      <c r="B18" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="C18" s="3">
         <v>1</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="5">
         <v>10</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="7"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="3">
         <v>2</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="5">
         <v>5</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="7"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="3">
         <v>3</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E20" s="5">
         <v>10</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="7" t="s">
-        <v>63</v>
+      <c r="B21" s="12" t="s">
+        <v>62</v>
       </c>
       <c r="C21" s="3">
         <v>1</v>
@@ -1068,7 +1064,7 @@
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="7"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="3">
         <v>2</v>
       </c>
@@ -1086,7 +1082,7 @@
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="3">
@@ -1099,14 +1095,14 @@
         <v>8</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="7"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="3">
         <v>2</v>
       </c>
@@ -1117,19 +1113,19 @@
         <v>5</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="7"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="3">
         <v>3</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>5</v>
@@ -1143,12 +1139,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B23:B25"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B8:B17"/>
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>